<commit_message>
Updated resources list with a few more resources
</commit_message>
<xml_diff>
--- a/resources/Resource List.xlsx
+++ b/resources/Resource List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater.sharepoint.com/sites/dwr-str/Shared Documents/IEP workshop 2024/Data Management Workshop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/GitHub/iep-data-workshop-2024/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="496" documentId="11_92B70280A3F276B9F3A2358F9CFCC713AAC2F873" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{386E9399-D479-42C1-9523-78E3D35E64FF}"/>
+  <xr:revisionPtr revIDLastSave="520" documentId="11_92B70280A3F276B9F3A2358F9CFCC713AAC2F873" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39231A3D-13C1-4EE6-BBFD-5E78123B0F78}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2520" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="172">
   <si>
     <t>Type</t>
   </si>
@@ -170,9 +170,6 @@
     <t>EMP Annual Report</t>
   </si>
   <si>
-    <t>https://emp-des.github.io/emp-reports/index.html</t>
-  </si>
-  <si>
     <t>IEP Seasonal Monitoring Report</t>
   </si>
   <si>
@@ -534,6 +531,27 @@
   </si>
   <si>
     <t>https://interagencyecologicalprogram.github.io/iep-data-workshop-2024/baydelta-figure-gallery.html</t>
+  </si>
+  <si>
+    <t>https://cadwr.app.box.com/v/InteragencyEcologicalProgram/folder/198778589381</t>
+  </si>
+  <si>
+    <t>DWR QA/QC documents and guidance</t>
+  </si>
+  <si>
+    <t>https://storymaps.arcgis.com/stories/d638a61723de4da583ab14ea71941be3</t>
+  </si>
+  <si>
+    <t>Smelt Supplementation StoryMap</t>
+  </si>
+  <si>
+    <t>https://storymaps.arcgis.com/stories/d0a9fdab3d534fada12b2dcca8bb0fe7</t>
+  </si>
+  <si>
+    <t>Shasta Reservoir StoryMap</t>
+  </si>
+  <si>
+    <t>https://emp-dwr.github.io/emp-website/</t>
   </si>
 </sst>
 </file>
@@ -923,11 +941,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,13 +1050,13 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" t="s">
         <v>148</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -1102,13 +1120,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
         <v>50</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1152,640 +1170,673 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" t="s">
-        <v>147</v>
+        <v>168</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" t="s">
-        <v>146</v>
+        <v>170</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>49</v>
+        <v>43</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>58</v>
+        <v>47</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
         <v>53</v>
       </c>
-      <c r="C20" t="s">
-        <v>59</v>
-      </c>
       <c r="D20" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
+      </c>
+      <c r="E23" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" t="s">
-        <v>63</v>
+        <v>68</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E27" t="s">
-        <v>77</v>
+        <v>70</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E28" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>62</v>
+        <v>74</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="E29" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
+      </c>
+      <c r="E30" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>85</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>81</v>
       </c>
       <c r="C32" t="s">
-        <v>87</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>88</v>
+        <v>82</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>137</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>138</v>
+        <v>91</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>93</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="C37" t="s">
-        <v>90</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>91</v>
+        <v>136</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>96</v>
-      </c>
-      <c r="B38" t="s">
-        <v>145</v>
+        <v>52</v>
       </c>
       <c r="C38" t="s">
-        <v>139</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E38" t="s">
-        <v>141</v>
+        <v>166</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>96</v>
-      </c>
-      <c r="B39" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C39" t="s">
-        <v>98</v>
+        <v>6</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>99</v>
+        <v>7</v>
+      </c>
+      <c r="F39" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>96</v>
-      </c>
-      <c r="B40" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C40" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B41" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C41" t="s">
-        <v>98</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>152</v>
+        <v>138</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E41" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" t="s">
         <v>96</v>
       </c>
-      <c r="B42" t="s">
-        <v>102</v>
-      </c>
       <c r="C42" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C43" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C44" t="s">
-        <v>154</v>
+        <v>97</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B45" t="s">
-        <v>156</v>
+        <v>101</v>
       </c>
       <c r="C45" t="s">
-        <v>159</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>162</v>
+        <v>102</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B46" t="s">
-        <v>157</v>
+        <v>101</v>
       </c>
       <c r="C46" t="s">
-        <v>160</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>163</v>
+        <v>102</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C47" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>106</v>
+        <v>95</v>
+      </c>
+      <c r="B48" t="s">
+        <v>155</v>
       </c>
       <c r="C48" t="s">
-        <v>107</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E48" t="s">
-        <v>13</v>
+        <v>158</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>109</v>
+        <v>95</v>
+      </c>
+      <c r="B49" t="s">
+        <v>156</v>
       </c>
       <c r="C49" t="s">
-        <v>110</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E49" t="s">
-        <v>112</v>
+        <v>159</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>109</v>
+        <v>95</v>
+      </c>
+      <c r="B50" t="s">
+        <v>157</v>
       </c>
       <c r="C50" t="s">
-        <v>113</v>
+        <v>160</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E50" t="s">
-        <v>56</v>
+        <v>163</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C51" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E51" t="s">
-        <v>135</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" t="s">
         <v>109</v>
       </c>
-      <c r="C52" t="s">
-        <v>117</v>
-      </c>
       <c r="D52" s="5" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E52" t="s">
-        <v>63</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>109</v>
-      </c>
-      <c r="B53" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C53" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>121</v>
+        <v>113</v>
+      </c>
+      <c r="E53" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>109</v>
-      </c>
-      <c r="B54" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="C54" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>144</v>
+        <v>115</v>
+      </c>
+      <c r="E54" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="C55" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>124</v>
+        <v>117</v>
+      </c>
+      <c r="E55" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>108</v>
+      </c>
+      <c r="B56" t="s">
+        <v>118</v>
       </c>
       <c r="C56" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>122</v>
+        <v>108</v>
+      </c>
+      <c r="B57" t="s">
+        <v>141</v>
       </c>
       <c r="C57" t="s">
-        <v>127</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>128</v>
+        <v>142</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>129</v>
-      </c>
-      <c r="B58" s="1"/>
+        <v>121</v>
+      </c>
       <c r="C58" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="E58" t="s">
-        <v>132</v>
-      </c>
-      <c r="F58" s="1"/>
+        <v>123</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>129</v>
-      </c>
-      <c r="B59" s="1"/>
+        <v>121</v>
+      </c>
       <c r="C59" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="E59" t="s">
-        <v>135</v>
-      </c>
-      <c r="F59" s="1"/>
+        <v>125</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" t="s">
+        <v>126</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>128</v>
+      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" t="s">
         <v>129</v>
       </c>
-      <c r="C60" t="s">
-        <v>136</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="E60" t="s">
-        <v>112</v>
+      <c r="D61" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E61" t="s">
+        <v>131</v>
+      </c>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>128</v>
+      </c>
+      <c r="B62" s="1"/>
+      <c r="C62" t="s">
+        <v>132</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E62" t="s">
+        <v>134</v>
+      </c>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" t="s">
+        <v>135</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E63" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:F60">
-    <sortCondition ref="A2:A60"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:F63">
+    <sortCondition ref="A2:A63"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="D39" r:id="rId1" xr:uid="{396CDDE7-EA37-430C-B2AE-95079A360CAC}"/>
-    <hyperlink ref="D40" r:id="rId2" xr:uid="{D2741F2A-B50F-433C-89BE-18E97F4E849C}"/>
-    <hyperlink ref="D48" r:id="rId3" xr:uid="{81918116-FFC7-4076-9FE3-7FADCDFD4F59}"/>
+    <hyperlink ref="D42" r:id="rId1" xr:uid="{396CDDE7-EA37-430C-B2AE-95079A360CAC}"/>
+    <hyperlink ref="D43" r:id="rId2" xr:uid="{D2741F2A-B50F-433C-89BE-18E97F4E849C}"/>
+    <hyperlink ref="D51" r:id="rId3" xr:uid="{81918116-FFC7-4076-9FE3-7FADCDFD4F59}"/>
     <hyperlink ref="D7" r:id="rId4" xr:uid="{A0A8670B-6FDB-4250-B863-4E52FC6E7742}"/>
-    <hyperlink ref="D23" r:id="rId5" xr:uid="{6DF79928-0FEB-493A-B4A2-B931DA2AED23}"/>
-    <hyperlink ref="D42" r:id="rId6" xr:uid="{9E548219-C7AA-43C6-B810-57A201C068FD}"/>
-    <hyperlink ref="D43" r:id="rId7" xr:uid="{E17BE5F2-11E0-4727-BA16-426C8929A062}"/>
+    <hyperlink ref="D25" r:id="rId5" xr:uid="{6DF79928-0FEB-493A-B4A2-B931DA2AED23}"/>
+    <hyperlink ref="D45" r:id="rId6" xr:uid="{9E548219-C7AA-43C6-B810-57A201C068FD}"/>
+    <hyperlink ref="D46" r:id="rId7" xr:uid="{E17BE5F2-11E0-4727-BA16-426C8929A062}"/>
     <hyperlink ref="D9" r:id="rId8" xr:uid="{D6B42CCB-0F33-46CF-9D4E-30CD7169C45B}"/>
     <hyperlink ref="D8" r:id="rId9" xr:uid="{F56AB587-3676-4FE2-A9C8-37A65FD89C2A}"/>
     <hyperlink ref="D10" r:id="rId10" xr:uid="{DC6C70A3-C20A-4FE8-A991-BF0D71CE109F}"/>
@@ -1793,76 +1844,59 @@
     <hyperlink ref="D3" r:id="rId12" xr:uid="{2861B25F-CC1F-463D-9687-432F842D2F23}"/>
     <hyperlink ref="D4" r:id="rId13" display="https://github.com/goertler/inundation" xr:uid="{F617B223-4747-492C-8462-A683169A2E72}"/>
     <hyperlink ref="D5" r:id="rId14" xr:uid="{DDC77059-4187-4D60-8C9F-C7D409C6C368}"/>
-    <hyperlink ref="D15" r:id="rId15" xr:uid="{87ECD766-0716-47F2-9112-2A7FB8D90883}"/>
-    <hyperlink ref="D16" r:id="rId16" xr:uid="{8D65757A-7BEF-4323-ABD1-551125078F9B}"/>
-    <hyperlink ref="D55" r:id="rId17" xr:uid="{52A12256-F3FC-4F0F-BBB1-FF5C0E99825B}"/>
-    <hyperlink ref="D56" r:id="rId18" xr:uid="{E4992D11-8FD6-45A3-937A-23B25F8A5A0D}"/>
-    <hyperlink ref="D36" r:id="rId19" xr:uid="{F769B676-A166-4BF5-99D1-E88EC28563CD}"/>
-    <hyperlink ref="D37" r:id="rId20" xr:uid="{801E0453-3D56-49EC-95FF-E5A7EA005F37}"/>
-    <hyperlink ref="D58" r:id="rId21" xr:uid="{58AFAE29-FC50-4EB8-B532-2077FA98F018}"/>
-    <hyperlink ref="D19" r:id="rId22" xr:uid="{6D3E2D77-4C7F-45E3-88B7-890543F60803}"/>
-    <hyperlink ref="E23" r:id="rId23" display="mailto:info@edirepository.org" xr:uid="{BC08C843-D313-4113-8053-C9CCD2F84BA9}"/>
-    <hyperlink ref="D29" r:id="rId24" xr:uid="{3FAC8B02-5A55-495A-9C09-1B8D11FD2E1C}"/>
-    <hyperlink ref="D59" r:id="rId25" xr:uid="{3B605933-B8BA-4A1E-ADB2-E4858AF5CC4E}"/>
-    <hyperlink ref="D28" r:id="rId26" xr:uid="{A33B077B-EFB7-47FF-85A9-40D90BF54838}"/>
-    <hyperlink ref="D30" r:id="rId27" xr:uid="{64AE0E96-A4F3-4D6A-A762-D44C70CE4300}"/>
-    <hyperlink ref="D22" r:id="rId28" xr:uid="{3E3026C1-2C5D-43E3-88DA-11AF57DB51AE}"/>
-    <hyperlink ref="D53" r:id="rId29" xr:uid="{EF584067-3777-4F2D-BDC6-45D5EB73B0AA}"/>
-    <hyperlink ref="D31" r:id="rId30" display="https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fdoc.arcgis.com%2Fen%2Farcgis-storymaps%2Fget-started%2Fauthor-and-publish-your-first-story.htm&amp;data=05%7C02%7Ccpien%40usbr.gov%7Cf469c29d9e7b4a0a37d408dc55b63c2b%7C0693b5ba4b184d7b9341f32f400a5494%7C0%7C0%7C638479488408533757%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C0%7C%7C%7C&amp;sdata=aNoV7mNZke27GjkIL5rFFRXqyIcFPgwOvSPb3DWYt88%3D&amp;reserved=0" xr:uid="{A8A197C8-0B44-4FAF-96BD-9CC0A6CEB8DF}"/>
-    <hyperlink ref="D32" r:id="rId31" display="https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Flearn.arcgis.com%2Fen%2Fpaths%2Fgetting-to-know-the-new-storymaps%2F&amp;data=05%7C02%7Ccpien%40usbr.gov%7Cf469c29d9e7b4a0a37d408dc55b63c2b%7C0693b5ba4b184d7b9341f32f400a5494%7C0%7C0%7C638479488408546255%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C0%7C%7C%7C&amp;sdata=Z4CNn3b8ALAFNiGRo9O81nU%2B60nIDwwj3myEFOHg5Ow%3D&amp;reserved=0" xr:uid="{6246FF79-325B-4804-B85C-B411D7BC4D4E}"/>
-    <hyperlink ref="D12" r:id="rId32" display="https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fstorymaps.arcgis.com%2Fstories%2Fa90f3b32b0b24f44a3fbc488f1e53bc3&amp;data=05%7C02%7Ccpien%40usbr.gov%7Cf469c29d9e7b4a0a37d408dc55b63c2b%7C0693b5ba4b184d7b9341f32f400a5494%7C0%7C0%7C638479488408553899%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C0%7C%7C%7C&amp;sdata=TEYEqJcfmZrnKbYT2Zh25ZelMu3sdNIlp%2FfZSggJDkI%3D&amp;reserved=0" xr:uid="{CCC87F1F-F146-4E75-8C7C-E13DEA989EE0}"/>
-    <hyperlink ref="D13" r:id="rId33" display="https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fstorymaps.arcgis.com%2Fstories%2F7369881210aa4403bea959676273dadb&amp;data=05%7C02%7Ccpien%40usbr.gov%7Cf469c29d9e7b4a0a37d408dc55b63c2b%7C0693b5ba4b184d7b9341f32f400a5494%7C0%7C0%7C638479488408564723%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C0%7C%7C%7C&amp;sdata=A3UFZQ51N3iCceGNVWNySVtCE%2B4iRkbDeDhXsekpwIQ%3D&amp;reserved=0" xr:uid="{42E6B353-D10C-4895-BECD-86E963791CBA}"/>
-    <hyperlink ref="D14" r:id="rId34" display="https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.arcgis.com%2Fapps%2FCascade%2Findex.html%3Fappid%3Dc5a9f0494c284f5fbf4d0150a0b7db2d&amp;data=05%7C02%7Ccpien%40usbr.gov%7Cf469c29d9e7b4a0a37d408dc55b63c2b%7C0693b5ba4b184d7b9341f32f400a5494%7C0%7C0%7C638479488408573713%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C0%7C%7C%7C&amp;sdata=wuK1hyAbNXqu90UahDnmXgAd51RrTNn5oAWMEss15g8%3D&amp;reserved=0" xr:uid="{33DC3AD9-0AC3-44C6-B6B4-C0E0836CB77F}"/>
-    <hyperlink ref="D21" r:id="rId35" xr:uid="{1CF45F52-D155-4AF6-B643-2809BA4BE60F}"/>
-    <hyperlink ref="D26" r:id="rId36" xr:uid="{D04E90E9-D912-4707-B4ED-D5C6306F3858}"/>
-    <hyperlink ref="D49" r:id="rId37" xr:uid="{1706ACBE-713E-42A5-81B7-8882B876A4A1}"/>
-    <hyperlink ref="D50" r:id="rId38" xr:uid="{3C7617F6-BB93-4BE6-912C-543E1D7F0DA1}"/>
-    <hyperlink ref="D51" r:id="rId39" xr:uid="{F4D9ACC4-5712-452B-B138-55D8A813FC1E}"/>
-    <hyperlink ref="D52" r:id="rId40" xr:uid="{BB024B52-69C1-488B-BA64-D35948912295}"/>
-    <hyperlink ref="D17" r:id="rId41" xr:uid="{336F5E73-FBF3-49F5-B8B5-4707758906E7}"/>
-    <hyperlink ref="D33" r:id="rId42" xr:uid="{5272D405-81D6-48BC-AC0B-7BA6FCA178AC}"/>
-    <hyperlink ref="D34" r:id="rId43" xr:uid="{D6C8BD13-6385-468E-8CCA-79C82B83871B}"/>
-    <hyperlink ref="D11" r:id="rId44" xr:uid="{B953C73C-C855-4DB0-8A1E-87D7B81BD090}"/>
-    <hyperlink ref="D24" r:id="rId45" xr:uid="{BE7906D1-F5C9-4014-962E-D407BBEC8919}"/>
-    <hyperlink ref="D25" r:id="rId46" xr:uid="{374BA80B-E0B9-4EBC-8669-0BBCCAF04DF7}"/>
-    <hyperlink ref="E24" r:id="rId47" display="mailto:info@edirepository.org" xr:uid="{F2B9C81F-9BE6-4756-AF13-F59F4869ABEC}"/>
-    <hyperlink ref="E25" r:id="rId48" display="mailto:info@edirepository.org" xr:uid="{6B8A812E-EEBF-4070-BF32-79F0DF3B1A27}"/>
-    <hyperlink ref="D35" r:id="rId49" xr:uid="{67C0405C-9496-44FA-BC8B-962A6A1D1091}"/>
-    <hyperlink ref="D38" r:id="rId50" xr:uid="{DB6C58C2-6C1E-4BF6-9277-D8F8714E8A0B}"/>
-    <hyperlink ref="D57" r:id="rId51" xr:uid="{D4254391-0E15-4F31-B3AE-8B2D41BEEFD4}"/>
-    <hyperlink ref="D27" r:id="rId52" xr:uid="{011AE430-3196-4566-A28B-6A850E881936}"/>
-    <hyperlink ref="D54" r:id="rId53" xr:uid="{090B9FAA-5C6A-4B17-9082-29151940DED8}"/>
-    <hyperlink ref="D45" r:id="rId54" xr:uid="{D59BABD9-D15E-459F-AE81-C72A63C61A3D}"/>
-    <hyperlink ref="D46" r:id="rId55" xr:uid="{6CBA211C-F728-476E-B73F-8B34577F10C1}"/>
-    <hyperlink ref="D47" r:id="rId56" xr:uid="{C71251EB-DD11-44CD-BABC-8AEC4D2AE110}"/>
-    <hyperlink ref="D60" r:id="rId57" xr:uid="{80A94DA0-626A-4BC0-9643-BD679BEE153A}"/>
+    <hyperlink ref="D18" r:id="rId15" xr:uid="{8D65757A-7BEF-4323-ABD1-551125078F9B}"/>
+    <hyperlink ref="D58" r:id="rId16" xr:uid="{52A12256-F3FC-4F0F-BBB1-FF5C0E99825B}"/>
+    <hyperlink ref="D59" r:id="rId17" xr:uid="{E4992D11-8FD6-45A3-937A-23B25F8A5A0D}"/>
+    <hyperlink ref="D39" r:id="rId18" xr:uid="{F769B676-A166-4BF5-99D1-E88EC28563CD}"/>
+    <hyperlink ref="D40" r:id="rId19" xr:uid="{801E0453-3D56-49EC-95FF-E5A7EA005F37}"/>
+    <hyperlink ref="D61" r:id="rId20" xr:uid="{58AFAE29-FC50-4EB8-B532-2077FA98F018}"/>
+    <hyperlink ref="D21" r:id="rId21" xr:uid="{6D3E2D77-4C7F-45E3-88B7-890543F60803}"/>
+    <hyperlink ref="E25" r:id="rId22" display="mailto:info@edirepository.org" xr:uid="{BC08C843-D313-4113-8053-C9CCD2F84BA9}"/>
+    <hyperlink ref="D31" r:id="rId23" xr:uid="{3FAC8B02-5A55-495A-9C09-1B8D11FD2E1C}"/>
+    <hyperlink ref="D62" r:id="rId24" xr:uid="{3B605933-B8BA-4A1E-ADB2-E4858AF5CC4E}"/>
+    <hyperlink ref="D30" r:id="rId25" xr:uid="{A33B077B-EFB7-47FF-85A9-40D90BF54838}"/>
+    <hyperlink ref="D32" r:id="rId26" xr:uid="{64AE0E96-A4F3-4D6A-A762-D44C70CE4300}"/>
+    <hyperlink ref="D24" r:id="rId27" xr:uid="{3E3026C1-2C5D-43E3-88DA-11AF57DB51AE}"/>
+    <hyperlink ref="D56" r:id="rId28" xr:uid="{EF584067-3777-4F2D-BDC6-45D5EB73B0AA}"/>
+    <hyperlink ref="D33" r:id="rId29" display="https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fdoc.arcgis.com%2Fen%2Farcgis-storymaps%2Fget-started%2Fauthor-and-publish-your-first-story.htm&amp;data=05%7C02%7Ccpien%40usbr.gov%7Cf469c29d9e7b4a0a37d408dc55b63c2b%7C0693b5ba4b184d7b9341f32f400a5494%7C0%7C0%7C638479488408533757%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C0%7C%7C%7C&amp;sdata=aNoV7mNZke27GjkIL5rFFRXqyIcFPgwOvSPb3DWYt88%3D&amp;reserved=0" xr:uid="{A8A197C8-0B44-4FAF-96BD-9CC0A6CEB8DF}"/>
+    <hyperlink ref="D34" r:id="rId30" display="https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Flearn.arcgis.com%2Fen%2Fpaths%2Fgetting-to-know-the-new-storymaps%2F&amp;data=05%7C02%7Ccpien%40usbr.gov%7Cf469c29d9e7b4a0a37d408dc55b63c2b%7C0693b5ba4b184d7b9341f32f400a5494%7C0%7C0%7C638479488408546255%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C0%7C%7C%7C&amp;sdata=Z4CNn3b8ALAFNiGRo9O81nU%2B60nIDwwj3myEFOHg5Ow%3D&amp;reserved=0" xr:uid="{6246FF79-325B-4804-B85C-B411D7BC4D4E}"/>
+    <hyperlink ref="D12" r:id="rId31" display="https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fstorymaps.arcgis.com%2Fstories%2Fa90f3b32b0b24f44a3fbc488f1e53bc3&amp;data=05%7C02%7Ccpien%40usbr.gov%7Cf469c29d9e7b4a0a37d408dc55b63c2b%7C0693b5ba4b184d7b9341f32f400a5494%7C0%7C0%7C638479488408553899%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C0%7C%7C%7C&amp;sdata=TEYEqJcfmZrnKbYT2Zh25ZelMu3sdNIlp%2FfZSggJDkI%3D&amp;reserved=0" xr:uid="{CCC87F1F-F146-4E75-8C7C-E13DEA989EE0}"/>
+    <hyperlink ref="D13" r:id="rId32" display="https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fstorymaps.arcgis.com%2Fstories%2F7369881210aa4403bea959676273dadb&amp;data=05%7C02%7Ccpien%40usbr.gov%7Cf469c29d9e7b4a0a37d408dc55b63c2b%7C0693b5ba4b184d7b9341f32f400a5494%7C0%7C0%7C638479488408564723%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C0%7C%7C%7C&amp;sdata=A3UFZQ51N3iCceGNVWNySVtCE%2B4iRkbDeDhXsekpwIQ%3D&amp;reserved=0" xr:uid="{42E6B353-D10C-4895-BECD-86E963791CBA}"/>
+    <hyperlink ref="D14" r:id="rId33" display="https://gcc02.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.arcgis.com%2Fapps%2FCascade%2Findex.html%3Fappid%3Dc5a9f0494c284f5fbf4d0150a0b7db2d&amp;data=05%7C02%7Ccpien%40usbr.gov%7Cf469c29d9e7b4a0a37d408dc55b63c2b%7C0693b5ba4b184d7b9341f32f400a5494%7C0%7C0%7C638479488408573713%7CUnknown%7CTWFpbGZsb3d8eyJWIjoiMC4wLjAwMDAiLCJQIjoiV2luMzIiLCJBTiI6Ik1haWwiLCJXVCI6Mn0%3D%7C0%7C%7C%7C&amp;sdata=wuK1hyAbNXqu90UahDnmXgAd51RrTNn5oAWMEss15g8%3D&amp;reserved=0" xr:uid="{33DC3AD9-0AC3-44C6-B6B4-C0E0836CB77F}"/>
+    <hyperlink ref="D23" r:id="rId34" xr:uid="{1CF45F52-D155-4AF6-B643-2809BA4BE60F}"/>
+    <hyperlink ref="D28" r:id="rId35" xr:uid="{D04E90E9-D912-4707-B4ED-D5C6306F3858}"/>
+    <hyperlink ref="D52" r:id="rId36" xr:uid="{1706ACBE-713E-42A5-81B7-8882B876A4A1}"/>
+    <hyperlink ref="D53" r:id="rId37" xr:uid="{3C7617F6-BB93-4BE6-912C-543E1D7F0DA1}"/>
+    <hyperlink ref="D54" r:id="rId38" xr:uid="{F4D9ACC4-5712-452B-B138-55D8A813FC1E}"/>
+    <hyperlink ref="D55" r:id="rId39" xr:uid="{BB024B52-69C1-488B-BA64-D35948912295}"/>
+    <hyperlink ref="D19" r:id="rId40" xr:uid="{336F5E73-FBF3-49F5-B8B5-4707758906E7}"/>
+    <hyperlink ref="D35" r:id="rId41" xr:uid="{5272D405-81D6-48BC-AC0B-7BA6FCA178AC}"/>
+    <hyperlink ref="D36" r:id="rId42" xr:uid="{D6C8BD13-6385-468E-8CCA-79C82B83871B}"/>
+    <hyperlink ref="D11" r:id="rId43" xr:uid="{B953C73C-C855-4DB0-8A1E-87D7B81BD090}"/>
+    <hyperlink ref="D26" r:id="rId44" xr:uid="{BE7906D1-F5C9-4014-962E-D407BBEC8919}"/>
+    <hyperlink ref="D27" r:id="rId45" xr:uid="{374BA80B-E0B9-4EBC-8669-0BBCCAF04DF7}"/>
+    <hyperlink ref="E26" r:id="rId46" display="mailto:info@edirepository.org" xr:uid="{F2B9C81F-9BE6-4756-AF13-F59F4869ABEC}"/>
+    <hyperlink ref="E27" r:id="rId47" display="mailto:info@edirepository.org" xr:uid="{6B8A812E-EEBF-4070-BF32-79F0DF3B1A27}"/>
+    <hyperlink ref="D37" r:id="rId48" xr:uid="{67C0405C-9496-44FA-BC8B-962A6A1D1091}"/>
+    <hyperlink ref="D41" r:id="rId49" xr:uid="{DB6C58C2-6C1E-4BF6-9277-D8F8714E8A0B}"/>
+    <hyperlink ref="D60" r:id="rId50" xr:uid="{D4254391-0E15-4F31-B3AE-8B2D41BEEFD4}"/>
+    <hyperlink ref="D29" r:id="rId51" xr:uid="{011AE430-3196-4566-A28B-6A850E881936}"/>
+    <hyperlink ref="D57" r:id="rId52" xr:uid="{090B9FAA-5C6A-4B17-9082-29151940DED8}"/>
+    <hyperlink ref="D48" r:id="rId53" xr:uid="{D59BABD9-D15E-459F-AE81-C72A63C61A3D}"/>
+    <hyperlink ref="D49" r:id="rId54" xr:uid="{6CBA211C-F728-476E-B73F-8B34577F10C1}"/>
+    <hyperlink ref="D50" r:id="rId55" xr:uid="{C71251EB-DD11-44CD-BABC-8AEC4D2AE110}"/>
+    <hyperlink ref="D63" r:id="rId56" xr:uid="{80A94DA0-626A-4BC0-9643-BD679BEE153A}"/>
+    <hyperlink ref="D38" r:id="rId57" tooltip="https://cadwr.app.box.com/v/interagencyecologicalprogram/folder/198778589381" xr:uid="{DF3EA150-89E9-4D8E-A37F-A9F7BC9694D2}"/>
+    <hyperlink ref="D15" r:id="rId58" xr:uid="{BF54A672-AC27-4BAF-B398-C9D5E32795F4}"/>
+    <hyperlink ref="D16" r:id="rId59" xr:uid="{8D8E1F6B-223E-4B81-A1B5-D59EE772DEB9}"/>
+    <hyperlink ref="D17" r:id="rId60" xr:uid="{E36CAF2F-544A-4850-B534-00E2002636F3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId58"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId61"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f60d4be9-3557-4154-8f7f-0f7fc20459a7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8b6ba10b-a228-4f4d-bf61-76f051627eb1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009C2CC601CF85AD4AAE2E8C1628370B4C" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="81d43700bbd5370bc97db83268c40a77">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8b6ba10b-a228-4f4d-bf61-76f051627eb1" xmlns:ns3="4fa31878-c15f-4cc2-b832-57ca6f3405c8" xmlns:ns4="f60d4be9-3557-4154-8f7f-0f7fc20459a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2f4e98d2ff7a2a20f42e5462f46da254" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="8b6ba10b-a228-4f4d-bf61-76f051627eb1"/>
@@ -2096,10 +2130,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f60d4be9-3557-4154-8f7f-0f7fc20459a7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8b6ba10b-a228-4f4d-bf61-76f051627eb1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FE7E9BA-7F12-4E6F-BD7F-560555F8CE5A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F1B83F2-396E-4971-9290-78B1FC3F3DE8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8b6ba10b-a228-4f4d-bf61-76f051627eb1"/>
+    <ds:schemaRef ds:uri="4fa31878-c15f-4cc2-b832-57ca6f3405c8"/>
+    <ds:schemaRef ds:uri="f60d4be9-3557-4154-8f7f-0f7fc20459a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2123,21 +2189,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F1B83F2-396E-4971-9290-78B1FC3F3DE8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FE7E9BA-7F12-4E6F-BD7F-560555F8CE5A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8b6ba10b-a228-4f4d-bf61-76f051627eb1"/>
-    <ds:schemaRef ds:uri="4fa31878-c15f-4cc2-b832-57ca6f3405c8"/>
-    <ds:schemaRef ds:uri="f60d4be9-3557-4154-8f7f-0f7fc20459a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>